<commit_message>
Added building exposure function. Updated test functions.
</commit_message>
<xml_diff>
--- a/examples/fiat_test/fiat_configuration.xlsx
+++ b/examples/fiat_test/fiat_configuration.xlsx
@@ -540,13 +540,13 @@
   <dimension ref="A1:Q98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="11" customWidth="1" style="2" min="1" max="1"/>
-    <col width="16.85546875" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
     <col width="18.28515625" customWidth="1" style="2" min="3" max="3"/>
     <col hidden="1" width="11.7109375" customWidth="1" style="2" min="4" max="4"/>
     <col hidden="1" width="13.7109375" customWidth="1" style="2" min="5" max="5"/>
@@ -560,12 +560,12 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>results</t>
+          <t>Root</t>
         </is>
       </c>
       <c r="H1" s="17" t="inlineStr">
         <is>
-          <t>currency</t>
+          <t>Currency</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
@@ -577,12 +577,12 @@
     <row r="2">
       <c r="B2" t="inlineStr">
         <is>
-          <t>Risk</t>
+          <t>D:\HydroMT\hydromt_fiat\examples\fiat_test</t>
         </is>
       </c>
       <c r="H2" s="17" t="inlineStr">
         <is>
-          <t>language</t>
+          <t>Language</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -594,18 +594,18 @@
     <row r="3">
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>hazard</t>
+          <t>Hazard</t>
         </is>
       </c>
       <c r="H3" s="1" t="n"/>
       <c r="I3" s="1" t="inlineStr">
         <is>
+          <t>Vulnerability</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>vulnerability</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>C:\Users\eilan_dk\DATA\repos\hydromt_fiat\examples\fiat_test\vulnerability</t>
         </is>
       </c>
     </row>
@@ -617,12 +617,12 @@
       </c>
       <c r="I4" s="17" t="inlineStr">
         <is>
+          <t>Exposure</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
           <t>exposure</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>C:\Users\eilan_dk\DATA\repos\hydromt_fiat\examples\fiat_test\exposure</t>
         </is>
       </c>
       <c r="K4" s="1" t="n"/>
@@ -634,73 +634,104 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>flooding</t>
+          <t>Flooding</t>
         </is>
       </c>
       <c r="I5" s="1" t="inlineStr">
         <is>
+          <t>Output</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
           <t>output</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>C:\Users\eilan_dk\DATA\repos\hydromt_fiat\examples\fiat_test\output</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>use (1/0)</t>
+          <t>Use (1/0)</t>
         </is>
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>category</t>
+          <t>Category</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>max_damage</t>
+          <t>Maximum Damage</t>
         </is>
       </c>
       <c r="D6" s="1" t="n"/>
       <c r="E6" s="1" t="n"/>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>function</t>
+          <t>Function</t>
         </is>
       </c>
       <c r="G6" s="1" t="n"/>
       <c r="H6" s="1" t="inlineStr">
         <is>
-          <t>map</t>
+          <t>Map</t>
         </is>
       </c>
       <c r="I6" s="1" t="inlineStr">
         <is>
-          <t>weight</t>
+          <t>Weight</t>
         </is>
       </c>
       <c r="J6" s="1" t="inlineStr">
         <is>
-          <t>raster</t>
+          <t>Raster</t>
         </is>
       </c>
       <c r="K6" s="1" t="inlineStr">
         <is>
-          <t>unit</t>
+          <t>Unit</t>
         </is>
       </c>
       <c r="L6" s="1" t="inlineStr">
         <is>
-          <t>landuse</t>
+          <t>Landuse</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="n"/>
-      <c r="B7" s="4" t="n"/>
+      <c r="A7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Buildings Value</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>exposure\buildings_value.tif</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="5" t="n"/>

</xml_diff>